<commit_message>
Started adding model classes and enumerations
</commit_message>
<xml_diff>
--- a/DTA Timesheet.xlsx
+++ b/DTA Timesheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Derek12\Websites\DylanTaylorArt\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E3B152E-7795-43A1-A1C6-1692ED80367C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2AAD44BC-39DB-44C3-B5D1-C11A13899439}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12810" xr2:uid="{60DF4AC3-BC03-4BD3-A93B-2AA258ECDB98}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>Task</t>
   </si>
@@ -69,6 +69,9 @@
   </si>
   <si>
     <t>Total</t>
+  </si>
+  <si>
+    <t>Added Model classes Graphics, Collections</t>
   </si>
 </sst>
 </file>
@@ -452,10 +455,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FF146F9C-C34C-42C9-A414-9BE0020E9CF3}">
-  <dimension ref="A1:C13"/>
+  <dimension ref="A1:C15"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -576,13 +579,27 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B13" s="5" t="s">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B12" s="4"/>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>13</v>
+      </c>
+      <c r="B13" s="4">
+        <v>43357</v>
+      </c>
+      <c r="C13" s="3">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B15" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C13" s="5">
-        <f>SUM(C2:C12)</f>
-        <v>4.7</v>
+      <c r="C15" s="5">
+        <f>SUM(C2:C14)</f>
+        <v>6.2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Changed Id to ID made no differenceto 1:M relationship
</commit_message>
<xml_diff>
--- a/DTA Timesheet.xlsx
+++ b/DTA Timesheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Derek12\Websites\DylanTaylorArt\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2AAD44BC-39DB-44C3-B5D1-C11A13899439}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A72881C-2149-4212-B0AC-E6ED58943255}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12810" xr2:uid="{60DF4AC3-BC03-4BD3-A93B-2AA258ECDB98}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>Task</t>
   </si>
@@ -72,6 +72,9 @@
   </si>
   <si>
     <t>Added Model classes Graphics, Collections</t>
+  </si>
+  <si>
+    <t>Added controllers and views of the database</t>
   </si>
 </sst>
 </file>
@@ -455,10 +458,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FF146F9C-C34C-42C9-A414-9BE0020E9CF3}">
-  <dimension ref="A1:C15"/>
+  <dimension ref="A1:C16"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -593,13 +596,24 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="15" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B15" s="5" t="s">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>14</v>
+      </c>
+      <c r="B14" s="4">
+        <v>43358</v>
+      </c>
+      <c r="C14" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B16" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C15" s="5">
-        <f>SUM(C2:C14)</f>
-        <v>6.2</v>
+      <c r="C16" s="5">
+        <f>SUM(C2:C15)</f>
+        <v>8.1999999999999993</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Adding images and prices
</commit_message>
<xml_diff>
--- a/DTA Timesheet.xlsx
+++ b/DTA Timesheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Derek12\Websites\DylanTaylorArt\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A72881C-2149-4212-B0AC-E6ED58943255}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7CE8620-B8B9-4D9D-B404-44387B57F0C2}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12810" xr2:uid="{60DF4AC3-BC03-4BD3-A93B-2AA258ECDB98}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t>Task</t>
   </si>
@@ -75,6 +75,12 @@
   </si>
   <si>
     <t>Added controllers and views of the database</t>
+  </si>
+  <si>
+    <t>Added all the 2008 data to a modified database</t>
+  </si>
+  <si>
+    <t>Modified web pages as suggested my Marting</t>
   </si>
 </sst>
 </file>
@@ -458,10 +464,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FF146F9C-C34C-42C9-A414-9BE0020E9CF3}">
-  <dimension ref="A1:C16"/>
+  <dimension ref="A1:C19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+    <sheetView tabSelected="1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -607,13 +613,38 @@
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B16" s="5" t="s">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B15" s="4"/>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>15</v>
+      </c>
+      <c r="B16" s="4">
+        <v>39709</v>
+      </c>
+      <c r="C16" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>16</v>
+      </c>
+      <c r="B17" s="4">
+        <v>39710</v>
+      </c>
+      <c r="C17" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B19" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C16" s="5">
-        <f>SUM(C2:C15)</f>
-        <v>8.1999999999999993</v>
+      <c r="C19" s="5">
+        <f>SUM(C2:C18)</f>
+        <v>11.2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated prices from 3 galleries
</commit_message>
<xml_diff>
--- a/DTA Timesheet.xlsx
+++ b/DTA Timesheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Derek12\Websites\DylanTaylorArt\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7CE8620-B8B9-4D9D-B404-44387B57F0C2}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A818C5D1-AEB5-4117-B063-EFE194F7D21F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12810" xr2:uid="{60DF4AC3-BC03-4BD3-A93B-2AA258ECDB98}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
   <si>
     <t>Task</t>
   </si>
@@ -80,7 +80,13 @@
     <t>Added all the 2008 data to a modified database</t>
   </si>
   <si>
-    <t>Modified web pages as suggested my Marting</t>
+    <t>Modified web pages as suggested my Martin</t>
+  </si>
+  <si>
+    <t>Added 2008 Images and prices</t>
+  </si>
+  <si>
+    <t>Added remaining graphics</t>
   </si>
 </sst>
 </file>
@@ -464,10 +470,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FF146F9C-C34C-42C9-A414-9BE0020E9CF3}">
-  <dimension ref="A1:C19"/>
+  <dimension ref="A1:C21"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -621,7 +627,7 @@
         <v>15</v>
       </c>
       <c r="B16" s="4">
-        <v>39709</v>
+        <v>43361</v>
       </c>
       <c r="C16" s="3">
         <v>2</v>
@@ -632,19 +638,41 @@
         <v>16</v>
       </c>
       <c r="B17" s="4">
-        <v>39710</v>
+        <v>43362</v>
       </c>
       <c r="C17" s="3">
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B19" s="5" t="s">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>17</v>
+      </c>
+      <c r="B18" s="4">
+        <v>43363</v>
+      </c>
+      <c r="C18" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>18</v>
+      </c>
+      <c r="B19" s="4">
+        <v>43364</v>
+      </c>
+      <c r="C19" s="3">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B21" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C19" s="5">
-        <f>SUM(C2:C18)</f>
-        <v>11.2</v>
+      <c r="C21" s="5">
+        <f>SUM(C2:C20)</f>
+        <v>14.7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Displayed the graphics sorted into collections
</commit_message>
<xml_diff>
--- a/DTA Timesheet.xlsx
+++ b/DTA Timesheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Derek12\Websites\DylanTaylorArt\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A818C5D1-AEB5-4117-B063-EFE194F7D21F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01C96404-19D4-4BB7-A5FB-ABBE1F6778F8}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12810" xr2:uid="{60DF4AC3-BC03-4BD3-A93B-2AA258ECDB98}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
   <si>
     <t>Task</t>
   </si>
@@ -87,6 +87,9 @@
   </si>
   <si>
     <t>Added remaining graphics</t>
+  </si>
+  <si>
+    <t>Updated prices</t>
   </si>
 </sst>
 </file>
@@ -470,10 +473,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FF146F9C-C34C-42C9-A414-9BE0020E9CF3}">
-  <dimension ref="A1:C21"/>
+  <dimension ref="A1:C22"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -666,13 +669,24 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="21" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B21" s="5" t="s">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>19</v>
+      </c>
+      <c r="B20" s="4">
+        <v>43364</v>
+      </c>
+      <c r="C20" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B22" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C21" s="5">
-        <f>SUM(C2:C20)</f>
-        <v>14.7</v>
+      <c r="C22" s="5">
+        <f>SUM(C2:C21)</f>
+        <v>15.7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Improved home collection page and added more data
</commit_message>
<xml_diff>
--- a/DTA Timesheet.xlsx
+++ b/DTA Timesheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Derek12\Websites\DylanTaylorArt\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01C96404-19D4-4BB7-A5FB-ABBE1F6778F8}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19266D04-B122-4DF0-A23D-115DDEC271E0}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12810" xr2:uid="{60DF4AC3-BC03-4BD3-A93B-2AA258ECDB98}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
   <si>
     <t>Task</t>
   </si>
@@ -90,6 +90,12 @@
   </si>
   <si>
     <t>Updated prices</t>
+  </si>
+  <si>
+    <t>Collections Home Page</t>
+  </si>
+  <si>
+    <t>Sorted graphics by collection</t>
   </si>
 </sst>
 </file>
@@ -473,10 +479,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FF146F9C-C34C-42C9-A414-9BE0020E9CF3}">
-  <dimension ref="A1:C22"/>
+  <dimension ref="A1:C24"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
+      <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -680,13 +686,35 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B22" s="5" t="s">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>21</v>
+      </c>
+      <c r="B21" s="4">
+        <v>43367</v>
+      </c>
+      <c r="C21" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>20</v>
+      </c>
+      <c r="B22" s="4">
+        <v>43368</v>
+      </c>
+      <c r="C22" s="3">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B24" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C22" s="5">
-        <f>SUM(C2:C21)</f>
-        <v>15.7</v>
+      <c r="C24" s="5">
+        <f>SUM(C2:C23)</f>
+        <v>19.2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added a link to the collections page
</commit_message>
<xml_diff>
--- a/DTA Timesheet.xlsx
+++ b/DTA Timesheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Derek12\Websites\DylanTaylorArt\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1BE7FC1E-11B0-4B79-853C-52AE07CDFB4B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1513F566-9411-4192-B7F7-4E48E61944FB}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12810" xr2:uid="{60DF4AC3-BC03-4BD3-A93B-2AA258ECDB98}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
   <si>
     <t>Task</t>
   </si>
@@ -99,6 +99,9 @@
   </si>
   <si>
     <t>All Images Added</t>
+  </si>
+  <si>
+    <t>Added database to the gallery page</t>
   </si>
 </sst>
 </file>
@@ -482,10 +485,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FF146F9C-C34C-42C9-A414-9BE0020E9CF3}">
-  <dimension ref="A1:C25"/>
+  <dimension ref="A1:C26"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A16" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="A24" sqref="A24"/>
+      <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -722,13 +725,24 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B25" s="5" t="s">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>23</v>
+      </c>
+      <c r="B24" s="4">
+        <v>43372</v>
+      </c>
+      <c r="C24" s="3">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B26" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C25" s="5">
-        <f>SUM(C2:C24)</f>
-        <v>20.2</v>
+      <c r="C26" s="5">
+        <f>SUM(C2:C25)</f>
+        <v>20.7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Minor corrections from Martin
</commit_message>
<xml_diff>
--- a/DTA Timesheet.xlsx
+++ b/DTA Timesheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Derek12\Websites\DylanTaylorArt\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1513F566-9411-4192-B7F7-4E48E61944FB}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E85ABD88-BF24-405E-BC25-D97EF85F3DBA}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12810" xr2:uid="{60DF4AC3-BC03-4BD3-A93B-2AA258ECDB98}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
   <si>
     <t>Task</t>
   </si>
@@ -102,6 +102,9 @@
   </si>
   <si>
     <t>Added database to the gallery page</t>
+  </si>
+  <si>
+    <t>Completed Home and About pages</t>
   </si>
 </sst>
 </file>
@@ -485,10 +488,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FF146F9C-C34C-42C9-A414-9BE0020E9CF3}">
-  <dimension ref="A1:C26"/>
+  <dimension ref="A1:C27"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A16" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="C25" sqref="C25"/>
+      <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -736,13 +739,24 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="26" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B26" s="5" t="s">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>24</v>
+      </c>
+      <c r="B25" s="4">
+        <v>43374</v>
+      </c>
+      <c r="C25" s="3">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B27" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C26" s="5">
-        <f>SUM(C2:C25)</f>
-        <v>20.7</v>
+      <c r="C27" s="5">
+        <f>SUM(C2:C26)</f>
+        <v>21.2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
completed on show page
</commit_message>
<xml_diff>
--- a/DTA Timesheet.xlsx
+++ b/DTA Timesheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Derek12\Websites\DylanTaylorArt\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E85ABD88-BF24-405E-BC25-D97EF85F3DBA}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2AC214F6-D4AF-4F89-8A2F-10802FAE28A3}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12810" xr2:uid="{60DF4AC3-BC03-4BD3-A93B-2AA258ECDB98}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
   <si>
     <t>Task</t>
   </si>
@@ -105,6 +105,9 @@
   </si>
   <si>
     <t>Completed Home and About pages</t>
+  </si>
+  <si>
+    <t>Made corrections and added one graphic</t>
   </si>
 </sst>
 </file>
@@ -488,10 +491,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FF146F9C-C34C-42C9-A414-9BE0020E9CF3}">
-  <dimension ref="A1:C27"/>
+  <dimension ref="A1:C28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="C26" sqref="C26"/>
+    <sheetView tabSelected="1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
+      <selection activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -750,13 +753,24 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="27" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B27" s="5" t="s">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>25</v>
+      </c>
+      <c r="B26" s="4">
+        <v>43346</v>
+      </c>
+      <c r="C26" s="3">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B28" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C27" s="5">
-        <f>SUM(C2:C26)</f>
-        <v>21.2</v>
+      <c r="C28" s="5">
+        <f>SUM(C2:C27)</f>
+        <v>21.7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Made changes after feedback from Martin on Shows
</commit_message>
<xml_diff>
--- a/DTA Timesheet.xlsx
+++ b/DTA Timesheet.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Derek12\Websites\DylanTaylorArt\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2AC214F6-D4AF-4F89-8A2F-10802FAE28A3}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2AB897DC-3319-4C9D-99FB-B1498A213ED4}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12810" xr2:uid="{60DF4AC3-BC03-4BD3-A93B-2AA258ECDB98}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
   <si>
     <t>Task</t>
   </si>
@@ -108,6 +108,12 @@
   </si>
   <si>
     <t>Made corrections and added one graphic</t>
+  </si>
+  <si>
+    <t>First draft of On Show page</t>
+  </si>
+  <si>
+    <t>Investigating the old domain name</t>
   </si>
 </sst>
 </file>
@@ -491,10 +497,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FF146F9C-C34C-42C9-A414-9BE0020E9CF3}">
-  <dimension ref="A1:C28"/>
+  <dimension ref="A1:C31"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="C27" sqref="C27"/>
+    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
+      <selection activeCell="C30" sqref="C30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -764,13 +770,41 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="28" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B28" s="5" t="s">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B27" s="4"/>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>26</v>
+      </c>
+      <c r="B28" s="4">
+        <v>43350</v>
+      </c>
+      <c r="C28" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>27</v>
+      </c>
+      <c r="B29" s="4">
+        <v>43357</v>
+      </c>
+      <c r="C29" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B30" s="4"/>
+    </row>
+    <row r="31" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B31" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C28" s="5">
-        <f>SUM(C2:C27)</f>
-        <v>21.7</v>
+      <c r="C31" s="5">
+        <f>SUM(C2:C29)</f>
+        <v>23.7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added two more images and meta tags
</commit_message>
<xml_diff>
--- a/DTA Timesheet.xlsx
+++ b/DTA Timesheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Derek12\Websites\DylanTaylorArt\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E722BE5-D7A3-4B59-AC00-4FED1BE5A477}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B6A9D35-9551-4ED0-870E-2438C439236F}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12810" xr2:uid="{60DF4AC3-BC03-4BD3-A93B-2AA258ECDB98}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="37">
   <si>
     <t>Task</t>
   </si>
@@ -129,6 +129,18 @@
   </si>
   <si>
     <t>TOTAL</t>
+  </si>
+  <si>
+    <t>Discount</t>
+  </si>
+  <si>
+    <t>PAID</t>
+  </si>
+  <si>
+    <t>Changing named servers to winhost</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Making changes to the data </t>
   </si>
 </sst>
 </file>
@@ -138,7 +150,7 @@
   <numFmts count="1">
     <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -161,8 +173,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -172,6 +191,17 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -226,11 +256,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -239,9 +270,6 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
@@ -258,15 +286,6 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="14" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="44" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -280,12 +299,28 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="2" applyBorder="1"/>
+    <xf numFmtId="14" fontId="3" fillId="3" borderId="3" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="3" fillId="3" borderId="3" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="2" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="44" fontId="3" fillId="3" borderId="3" xfId="2" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="2" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
+    <cellStyle name="Good" xfId="2" builtinId="26"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -598,457 +633,503 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FF146F9C-C34C-42C9-A414-9BE0020E9CF3}">
-  <dimension ref="A1:F33"/>
+  <dimension ref="A1:G35"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
+      <selection activeCell="D27" sqref="D27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="43.85546875" customWidth="1"/>
     <col min="2" max="2" width="14.85546875" style="2" customWidth="1"/>
-    <col min="3" max="3" width="9.140625" style="22"/>
-    <col min="4" max="4" width="9.140625" style="7"/>
+    <col min="3" max="3" width="9.140625" style="16"/>
+    <col min="4" max="4" width="9.140625" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="18" t="s">
+    <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="19" t="s">
+      <c r="B1" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="C1" s="21" t="s">
+      <c r="C1" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="20" t="s">
+      <c r="D1" s="14" t="s">
         <v>30</v>
       </c>
-      <c r="E1" s="18" t="s">
+      <c r="E1" s="12" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="8" t="s">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="9">
+      <c r="B2" s="8">
         <v>43355</v>
       </c>
-      <c r="C2" s="12">
+      <c r="C2" s="11">
         <v>0.25</v>
       </c>
-      <c r="D2" s="10">
-        <v>25</v>
-      </c>
-      <c r="E2" s="11">
+      <c r="D2" s="9">
+        <v>25</v>
+      </c>
+      <c r="E2" s="10">
         <f t="shared" ref="E2:E11" si="0">D2*C2</f>
         <v>6.25</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="8" t="s">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="9">
+      <c r="B3" s="8">
         <v>43355</v>
       </c>
-      <c r="C3" s="12">
+      <c r="C3" s="11">
         <v>0.1</v>
       </c>
-      <c r="D3" s="10">
-        <v>25</v>
-      </c>
-      <c r="E3" s="11">
+      <c r="D3" s="9">
+        <v>25</v>
+      </c>
+      <c r="E3" s="10">
         <f t="shared" si="0"/>
         <v>2.5</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="8" t="s">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="9">
+      <c r="B4" s="8">
         <v>43355</v>
       </c>
-      <c r="C4" s="12">
+      <c r="C4" s="11">
         <v>0.25</v>
       </c>
-      <c r="D4" s="10">
-        <v>25</v>
-      </c>
-      <c r="E4" s="11">
+      <c r="D4" s="9">
+        <v>25</v>
+      </c>
+      <c r="E4" s="10">
         <f t="shared" si="0"/>
         <v>6.25</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="8" t="s">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="9">
+      <c r="B5" s="8">
         <v>43355</v>
       </c>
-      <c r="C5" s="12">
+      <c r="C5" s="11">
         <v>0.25</v>
       </c>
-      <c r="D5" s="10">
-        <v>25</v>
-      </c>
-      <c r="E5" s="11">
+      <c r="D5" s="9">
+        <v>25</v>
+      </c>
+      <c r="E5" s="10">
         <f t="shared" si="0"/>
         <v>6.25</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="8" t="s">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="9">
+      <c r="B6" s="8">
         <v>43355</v>
       </c>
-      <c r="C6" s="12">
+      <c r="C6" s="11">
         <v>0.1</v>
       </c>
-      <c r="D6" s="10">
-        <v>25</v>
-      </c>
-      <c r="E6" s="11">
+      <c r="D6" s="9">
+        <v>25</v>
+      </c>
+      <c r="E6" s="10">
         <f t="shared" si="0"/>
         <v>2.5</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="8" t="s">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="B7" s="9">
+      <c r="B7" s="8">
         <v>43355</v>
       </c>
-      <c r="C7" s="12">
+      <c r="C7" s="11">
         <v>0.25</v>
       </c>
-      <c r="D7" s="10">
-        <v>25</v>
-      </c>
-      <c r="E7" s="11">
+      <c r="D7" s="9">
+        <v>25</v>
+      </c>
+      <c r="E7" s="10">
         <f t="shared" si="0"/>
         <v>6.25</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="8" t="s">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="B8" s="9">
+      <c r="B8" s="8">
         <v>43355</v>
       </c>
-      <c r="C8" s="12">
+      <c r="C8" s="11">
         <v>0.5</v>
       </c>
-      <c r="D8" s="10">
-        <v>25</v>
-      </c>
-      <c r="E8" s="11">
+      <c r="D8" s="9">
+        <v>25</v>
+      </c>
+      <c r="E8" s="10">
         <f t="shared" si="0"/>
         <v>12.5</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="8" t="s">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="B9" s="9">
+      <c r="B9" s="8">
         <v>43356</v>
       </c>
-      <c r="C9" s="12">
+      <c r="C9" s="11">
         <v>2</v>
       </c>
-      <c r="D9" s="10">
-        <v>25</v>
-      </c>
-      <c r="E9" s="11">
+      <c r="D9" s="9">
+        <v>25</v>
+      </c>
+      <c r="E9" s="10">
         <f t="shared" si="0"/>
         <v>50</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="8" t="s">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="B10" s="9">
+      <c r="B10" s="8">
         <v>43356</v>
       </c>
-      <c r="C10" s="12">
+      <c r="C10" s="11">
         <v>1</v>
       </c>
-      <c r="D10" s="10">
-        <v>25</v>
-      </c>
-      <c r="E10" s="11">
+      <c r="D10" s="9">
+        <v>25</v>
+      </c>
+      <c r="E10" s="10">
         <f t="shared" si="0"/>
         <v>25</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="8" t="s">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="B11" s="9">
+      <c r="B11" s="8">
         <v>43357</v>
       </c>
-      <c r="C11" s="12">
+      <c r="C11" s="11">
         <v>1.5</v>
       </c>
-      <c r="D11" s="10">
-        <v>25</v>
-      </c>
-      <c r="E11" s="11">
+      <c r="D11" s="9">
+        <v>25</v>
+      </c>
+      <c r="E11" s="10">
         <f t="shared" si="0"/>
         <v>37.5</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="8" t="s">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="B12" s="9">
+      <c r="B12" s="8">
         <v>43358</v>
       </c>
-      <c r="C12" s="12">
+      <c r="C12" s="11">
         <v>2</v>
       </c>
-      <c r="D12" s="10">
-        <v>25</v>
-      </c>
-      <c r="E12" s="11">
+      <c r="D12" s="9">
+        <v>25</v>
+      </c>
+      <c r="E12" s="10">
         <f>D12*C12</f>
         <v>50</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" s="8" t="s">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="B13" s="9">
+      <c r="B13" s="8">
         <v>43361</v>
       </c>
-      <c r="C13" s="12">
+      <c r="C13" s="11">
         <v>2</v>
       </c>
-      <c r="D13" s="10">
-        <v>25</v>
-      </c>
-      <c r="E13" s="11">
+      <c r="D13" s="9">
+        <v>25</v>
+      </c>
+      <c r="E13" s="10">
         <f t="shared" ref="E13:E15" si="1">D13*C13</f>
         <v>50</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" s="8" t="s">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="B14" s="9">
+      <c r="B14" s="8">
         <v>43362</v>
       </c>
-      <c r="C14" s="12">
+      <c r="C14" s="11">
         <v>1</v>
       </c>
-      <c r="D14" s="10">
-        <v>25</v>
-      </c>
-      <c r="E14" s="11">
+      <c r="D14" s="9">
+        <v>25</v>
+      </c>
+      <c r="E14" s="10">
         <f t="shared" si="1"/>
         <v>25</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" s="8" t="s">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="B15" s="9">
+      <c r="B15" s="8">
         <v>43363</v>
       </c>
-      <c r="C15" s="12">
+      <c r="C15" s="11">
         <v>2</v>
       </c>
-      <c r="D15" s="10">
-        <v>25</v>
-      </c>
-      <c r="E15" s="11">
+      <c r="D15" s="9">
+        <v>25</v>
+      </c>
+      <c r="E15" s="10">
         <f t="shared" si="1"/>
         <v>50</v>
       </c>
     </row>
-    <row r="16" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="13"/>
-      <c r="B16" s="14" t="s">
+    <row r="16" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="17"/>
+      <c r="B16" s="18" t="s">
         <v>32</v>
       </c>
-      <c r="C16" s="15">
+      <c r="C16" s="19">
         <f>SUM(C2:C15)</f>
         <v>13.2</v>
       </c>
-      <c r="D16" s="16"/>
-      <c r="E16" s="17">
+      <c r="D16" s="20"/>
+      <c r="E16" s="21">
         <f>SUM(E2:E15)</f>
         <v>330</v>
       </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F16" s="22" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B17" s="3"/>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B18" s="3"/>
-      <c r="E18" s="5"/>
-      <c r="F18" s="6"/>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="B18" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="C18" s="15" t="s">
+        <v>1</v>
+      </c>
+      <c r="D18" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="E18" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="F18" s="5"/>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>18</v>
       </c>
       <c r="B19" s="3">
         <v>43364</v>
       </c>
-      <c r="C19" s="22">
+      <c r="C19" s="16">
         <v>1.5</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>19</v>
       </c>
       <c r="B20" s="3">
         <v>43364</v>
       </c>
-      <c r="C20" s="22">
+      <c r="C20" s="16">
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>21</v>
       </c>
       <c r="B21" s="3">
         <v>43367</v>
       </c>
-      <c r="C21" s="22">
+      <c r="C21" s="16">
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>20</v>
       </c>
       <c r="B22" s="3">
         <v>43368</v>
       </c>
-      <c r="C22" s="22">
+      <c r="C22" s="16">
         <v>2.5</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>22</v>
       </c>
       <c r="B23" s="3">
         <v>43369</v>
       </c>
-      <c r="C23" s="22">
+      <c r="C23" s="16">
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>23</v>
       </c>
       <c r="B24" s="3">
         <v>43372</v>
       </c>
-      <c r="C24" s="22">
+      <c r="C24" s="16">
         <v>0.5</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>24</v>
       </c>
       <c r="B25" s="3">
         <v>43374</v>
       </c>
-      <c r="C25" s="22">
+      <c r="C25" s="16">
         <v>0.5</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>25</v>
       </c>
       <c r="B26" s="3">
         <v>43376</v>
       </c>
-      <c r="C26" s="22">
+      <c r="C26" s="16">
         <v>0.5</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B27" s="3"/>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>26</v>
       </c>
       <c r="B28" s="3">
         <v>43380</v>
       </c>
-      <c r="C28" s="22">
+      <c r="C28" s="16">
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>27</v>
       </c>
       <c r="B29" s="3">
         <v>43387</v>
       </c>
-      <c r="C29" s="22">
+      <c r="C29" s="16">
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>28</v>
       </c>
       <c r="B30" s="3">
         <v>43388</v>
       </c>
-      <c r="C30" s="22">
+      <c r="C30" s="16">
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>29</v>
       </c>
       <c r="B31" s="3">
         <v>43753</v>
       </c>
-      <c r="C31" s="22">
+      <c r="C31" s="16">
         <v>0.5</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B32" s="3"/>
-    </row>
-    <row r="33" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B33" s="4" t="s">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>35</v>
+      </c>
+      <c r="B32" s="3">
+        <v>43392</v>
+      </c>
+      <c r="C32" s="16">
+        <v>0.5</v>
+      </c>
+      <c r="F32" s="4">
+        <v>35</v>
+      </c>
+      <c r="G32" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>36</v>
+      </c>
+      <c r="B33" s="3">
+        <v>43393</v>
+      </c>
+      <c r="C33" s="16">
+        <v>0.5</v>
+      </c>
+      <c r="F33" s="4"/>
+      <c r="G33" s="2"/>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B34" s="3"/>
+    </row>
+    <row r="35" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B35" s="23" t="s">
         <v>12</v>
       </c>
-      <c r="C33" s="23">
-        <f>SUM(C2:C31)</f>
-        <v>38.4</v>
+      <c r="C35" s="24">
+        <f>SUM(C19:C33)</f>
+        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Have added open graph protocol for twitter
</commit_message>
<xml_diff>
--- a/DTA Timesheet.xlsx
+++ b/DTA Timesheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Derek12\Websites\DylanTaylorArt\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B6A9D35-9551-4ED0-870E-2438C439236F}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84DBDE83-CF1F-4209-BEA4-4C7952009BF7}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12810" xr2:uid="{60DF4AC3-BC03-4BD3-A93B-2AA258ECDB98}"/>
   </bookViews>
@@ -29,8 +29,42 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Derek Peacock</author>
+  </authors>
+  <commentList>
+    <comment ref="A35" authorId="0" shapeId="0" xr:uid="{11EEC46F-A1D6-488F-9346-11C8A49BD9DD}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Derek Peacock:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+on 1and1.co.uk</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="41">
   <si>
     <t>Task</t>
   </si>
@@ -131,9 +165,6 @@
     <t>TOTAL</t>
   </si>
   <si>
-    <t>Discount</t>
-  </si>
-  <si>
     <t>PAID</t>
   </si>
   <si>
@@ -141,6 +172,21 @@
   </si>
   <si>
     <t xml:space="preserve">Making changes to the data </t>
+  </si>
+  <si>
+    <t>Publishing on dta.com and corrections</t>
+  </si>
+  <si>
+    <t>Coaching Discount</t>
+  </si>
+  <si>
+    <t>Purchasing Web Hosting on Winhost (1year)</t>
+  </si>
+  <si>
+    <t>Purchasing dta.co.uk domain name (2 years)</t>
+  </si>
+  <si>
+    <t>Corrections to the data</t>
   </si>
 </sst>
 </file>
@@ -150,7 +196,7 @@
   <numFmts count="1">
     <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -180,8 +226,43 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C5700"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -201,28 +282,21 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.39997558519241921"/>
-        <bgColor indexed="64"/>
+        <fgColor rgb="FFFFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="3">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -256,12 +330,14 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -275,52 +351,70 @@
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="1" fillId="2" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="1" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="1" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="2" applyBorder="1"/>
-    <xf numFmtId="14" fontId="3" fillId="3" borderId="3" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="3" fillId="3" borderId="3" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="2" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="44" fontId="3" fillId="3" borderId="3" xfId="2" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="2" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="2" applyBorder="1"/>
+    <xf numFmtId="14" fontId="6" fillId="3" borderId="2" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="6" fillId="3" borderId="2" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="2" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="44" fontId="6" fillId="3" borderId="2" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="44" fontId="4" fillId="4" borderId="1" xfId="3" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="4" applyBorder="1"/>
+    <xf numFmtId="14" fontId="5" fillId="5" borderId="1" xfId="4" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="5" fillId="5" borderId="1" xfId="4" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="5" fillId="5" borderId="1" xfId="4" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="5" fillId="5" borderId="1" xfId="4" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="2" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="5">
+    <cellStyle name="Bad" xfId="3" builtinId="27"/>
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
     <cellStyle name="Good" xfId="2" builtinId="26"/>
+    <cellStyle name="Neutral" xfId="4" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -632,11 +726,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FF146F9C-C34C-42C9-A414-9BE0020E9CF3}">
-  <dimension ref="A1:G35"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FF146F9C-C34C-42C9-A414-9BE0020E9CF3}">
+  <dimension ref="A1:G41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="D27" sqref="D27"/>
+    <sheetView tabSelected="1" topLeftCell="A18" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="G25" sqref="G25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -665,253 +759,253 @@
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="7" t="s">
+      <c r="A2" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="8">
+      <c r="B2" s="28">
         <v>43355</v>
       </c>
-      <c r="C2" s="11">
+      <c r="C2" s="29">
         <v>0.25</v>
       </c>
-      <c r="D2" s="9">
-        <v>25</v>
-      </c>
-      <c r="E2" s="10">
+      <c r="D2" s="30">
+        <v>25</v>
+      </c>
+      <c r="E2" s="31">
         <f t="shared" ref="E2:E11" si="0">D2*C2</f>
         <v>6.25</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="7" t="s">
+      <c r="A3" s="27" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="8">
+      <c r="B3" s="28">
         <v>43355</v>
       </c>
-      <c r="C3" s="11">
+      <c r="C3" s="29">
         <v>0.1</v>
       </c>
-      <c r="D3" s="9">
-        <v>25</v>
-      </c>
-      <c r="E3" s="10">
+      <c r="D3" s="30">
+        <v>25</v>
+      </c>
+      <c r="E3" s="31">
         <f t="shared" si="0"/>
         <v>2.5</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="7" t="s">
+      <c r="A4" s="27" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="8">
+      <c r="B4" s="28">
         <v>43355</v>
       </c>
-      <c r="C4" s="11">
+      <c r="C4" s="29">
         <v>0.25</v>
       </c>
-      <c r="D4" s="9">
-        <v>25</v>
-      </c>
-      <c r="E4" s="10">
+      <c r="D4" s="30">
+        <v>25</v>
+      </c>
+      <c r="E4" s="31">
         <f t="shared" si="0"/>
         <v>6.25</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="7" t="s">
+      <c r="A5" s="27" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="8">
+      <c r="B5" s="28">
         <v>43355</v>
       </c>
-      <c r="C5" s="11">
+      <c r="C5" s="29">
         <v>0.25</v>
       </c>
-      <c r="D5" s="9">
-        <v>25</v>
-      </c>
-      <c r="E5" s="10">
+      <c r="D5" s="30">
+        <v>25</v>
+      </c>
+      <c r="E5" s="31">
         <f t="shared" si="0"/>
         <v>6.25</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="7" t="s">
+      <c r="A6" s="27" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="8">
+      <c r="B6" s="28">
         <v>43355</v>
       </c>
-      <c r="C6" s="11">
+      <c r="C6" s="29">
         <v>0.1</v>
       </c>
-      <c r="D6" s="9">
-        <v>25</v>
-      </c>
-      <c r="E6" s="10">
+      <c r="D6" s="30">
+        <v>25</v>
+      </c>
+      <c r="E6" s="31">
         <f t="shared" si="0"/>
         <v>2.5</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="7" t="s">
+      <c r="A7" s="27" t="s">
         <v>8</v>
       </c>
-      <c r="B7" s="8">
+      <c r="B7" s="28">
         <v>43355</v>
       </c>
-      <c r="C7" s="11">
+      <c r="C7" s="29">
         <v>0.25</v>
       </c>
-      <c r="D7" s="9">
-        <v>25</v>
-      </c>
-      <c r="E7" s="10">
+      <c r="D7" s="30">
+        <v>25</v>
+      </c>
+      <c r="E7" s="31">
         <f t="shared" si="0"/>
         <v>6.25</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="7" t="s">
+      <c r="A8" s="27" t="s">
         <v>9</v>
       </c>
-      <c r="B8" s="8">
+      <c r="B8" s="28">
         <v>43355</v>
       </c>
-      <c r="C8" s="11">
+      <c r="C8" s="29">
         <v>0.5</v>
       </c>
-      <c r="D8" s="9">
-        <v>25</v>
-      </c>
-      <c r="E8" s="10">
+      <c r="D8" s="30">
+        <v>25</v>
+      </c>
+      <c r="E8" s="31">
         <f t="shared" si="0"/>
         <v>12.5</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="7" t="s">
+      <c r="A9" s="27" t="s">
         <v>10</v>
       </c>
-      <c r="B9" s="8">
+      <c r="B9" s="28">
         <v>43356</v>
       </c>
-      <c r="C9" s="11">
+      <c r="C9" s="29">
         <v>2</v>
       </c>
-      <c r="D9" s="9">
-        <v>25</v>
-      </c>
-      <c r="E9" s="10">
+      <c r="D9" s="30">
+        <v>25</v>
+      </c>
+      <c r="E9" s="31">
         <f t="shared" si="0"/>
         <v>50</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="7" t="s">
+      <c r="A10" s="27" t="s">
         <v>11</v>
       </c>
-      <c r="B10" s="8">
+      <c r="B10" s="28">
         <v>43356</v>
       </c>
-      <c r="C10" s="11">
+      <c r="C10" s="29">
         <v>1</v>
       </c>
-      <c r="D10" s="9">
-        <v>25</v>
-      </c>
-      <c r="E10" s="10">
+      <c r="D10" s="30">
+        <v>25</v>
+      </c>
+      <c r="E10" s="31">
         <f t="shared" si="0"/>
         <v>25</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" s="7" t="s">
+      <c r="A11" s="27" t="s">
         <v>13</v>
       </c>
-      <c r="B11" s="8">
+      <c r="B11" s="28">
         <v>43357</v>
       </c>
-      <c r="C11" s="11">
+      <c r="C11" s="29">
         <v>1.5</v>
       </c>
-      <c r="D11" s="9">
-        <v>25</v>
-      </c>
-      <c r="E11" s="10">
+      <c r="D11" s="30">
+        <v>25</v>
+      </c>
+      <c r="E11" s="31">
         <f t="shared" si="0"/>
         <v>37.5</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" s="7" t="s">
+      <c r="A12" s="27" t="s">
         <v>14</v>
       </c>
-      <c r="B12" s="8">
+      <c r="B12" s="28">
         <v>43358</v>
       </c>
-      <c r="C12" s="11">
+      <c r="C12" s="29">
         <v>2</v>
       </c>
-      <c r="D12" s="9">
-        <v>25</v>
-      </c>
-      <c r="E12" s="10">
+      <c r="D12" s="30">
+        <v>25</v>
+      </c>
+      <c r="E12" s="31">
         <f>D12*C12</f>
         <v>50</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" s="7" t="s">
+      <c r="A13" s="27" t="s">
         <v>15</v>
       </c>
-      <c r="B13" s="8">
+      <c r="B13" s="28">
         <v>43361</v>
       </c>
-      <c r="C13" s="11">
+      <c r="C13" s="29">
         <v>2</v>
       </c>
-      <c r="D13" s="9">
-        <v>25</v>
-      </c>
-      <c r="E13" s="10">
+      <c r="D13" s="30">
+        <v>25</v>
+      </c>
+      <c r="E13" s="31">
         <f t="shared" ref="E13:E15" si="1">D13*C13</f>
         <v>50</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" s="7" t="s">
+      <c r="A14" s="27" t="s">
         <v>16</v>
       </c>
-      <c r="B14" s="8">
+      <c r="B14" s="28">
         <v>43362</v>
       </c>
-      <c r="C14" s="11">
+      <c r="C14" s="29">
         <v>1</v>
       </c>
-      <c r="D14" s="9">
-        <v>25</v>
-      </c>
-      <c r="E14" s="10">
+      <c r="D14" s="30">
+        <v>25</v>
+      </c>
+      <c r="E14" s="31">
         <f t="shared" si="1"/>
         <v>25</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" s="7" t="s">
+      <c r="A15" s="27" t="s">
         <v>17</v>
       </c>
-      <c r="B15" s="8">
+      <c r="B15" s="28">
         <v>43363</v>
       </c>
-      <c r="C15" s="11">
+      <c r="C15" s="29">
         <v>2</v>
       </c>
-      <c r="D15" s="9">
-        <v>25</v>
-      </c>
-      <c r="E15" s="10">
+      <c r="D15" s="30">
+        <v>25</v>
+      </c>
+      <c r="E15" s="31">
         <f t="shared" si="1"/>
         <v>50</v>
       </c>
@@ -930,14 +1024,14 @@
         <f>SUM(E2:E15)</f>
         <v>330</v>
       </c>
-      <c r="F16" s="22" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F16" s="26" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B17" s="3"/>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="12" t="s">
         <v>0</v>
       </c>
@@ -955,185 +1049,381 @@
       </c>
       <c r="F18" s="5"/>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="B19" s="3">
+      <c r="B19" s="8">
         <v>43364</v>
       </c>
-      <c r="C19" s="16">
+      <c r="C19" s="11">
         <v>1.5</v>
       </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
+      <c r="D19" s="9">
+        <v>25</v>
+      </c>
+      <c r="E19" s="10">
+        <f>D19*C19</f>
+        <v>37.5</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="B20" s="3">
+      <c r="B20" s="8">
         <v>43364</v>
       </c>
-      <c r="C20" s="16">
+      <c r="C20" s="11">
         <v>1</v>
       </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
+      <c r="D20" s="9">
+        <v>25</v>
+      </c>
+      <c r="E20" s="10">
+        <f t="shared" ref="E20:E26" si="2">D20*C20</f>
+        <v>25</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="B21" s="3">
+      <c r="B21" s="8">
         <v>43367</v>
       </c>
-      <c r="C21" s="16">
+      <c r="C21" s="11">
         <v>1</v>
       </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
+      <c r="D21" s="9">
+        <v>25</v>
+      </c>
+      <c r="E21" s="10">
+        <f t="shared" si="2"/>
+        <v>25</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A22" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="B22" s="3">
+      <c r="B22" s="8">
         <v>43368</v>
       </c>
-      <c r="C22" s="16">
+      <c r="C22" s="11">
         <v>2.5</v>
       </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
+      <c r="D22" s="9">
+        <v>25</v>
+      </c>
+      <c r="E22" s="10">
+        <f t="shared" si="2"/>
+        <v>62.5</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A23" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="B23" s="3">
+      <c r="B23" s="8">
         <v>43369</v>
       </c>
-      <c r="C23" s="16">
+      <c r="C23" s="11">
         <v>1</v>
       </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
+      <c r="D23" s="9">
+        <v>25</v>
+      </c>
+      <c r="E23" s="10">
+        <f t="shared" si="2"/>
+        <v>25</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A24" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="B24" s="3">
+      <c r="B24" s="8">
         <v>43372</v>
       </c>
-      <c r="C24" s="16">
+      <c r="C24" s="11">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
+      <c r="D24" s="9">
+        <v>25</v>
+      </c>
+      <c r="E24" s="10">
+        <f t="shared" si="2"/>
+        <v>12.5</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A25" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="B25" s="3">
+      <c r="B25" s="8">
         <v>43374</v>
       </c>
-      <c r="C25" s="16">
+      <c r="C25" s="11">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
-        <v>25</v>
-      </c>
-      <c r="B26" s="3">
+      <c r="D25" s="9">
+        <v>25</v>
+      </c>
+      <c r="E25" s="10">
+        <f t="shared" si="2"/>
+        <v>12.5</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A26" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="B26" s="8">
         <v>43376</v>
       </c>
-      <c r="C26" s="16">
+      <c r="C26" s="11">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B27" s="3"/>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
+      <c r="D26" s="9">
+        <v>25</v>
+      </c>
+      <c r="E26" s="10">
+        <f t="shared" si="2"/>
+        <v>12.5</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A27" s="7"/>
+      <c r="B27" s="8"/>
+      <c r="C27" s="11"/>
+      <c r="D27" s="9"/>
+      <c r="E27" s="7"/>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A28" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="B28" s="3">
+      <c r="B28" s="8">
         <v>43380</v>
       </c>
-      <c r="C28" s="16">
+      <c r="C28" s="11">
         <v>1</v>
       </c>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
+      <c r="D28" s="9">
+        <v>25</v>
+      </c>
+      <c r="E28" s="10">
+        <f>D28*C28</f>
+        <v>25</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A29" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="B29" s="3">
+      <c r="B29" s="8">
         <v>43387</v>
       </c>
-      <c r="C29" s="16">
+      <c r="C29" s="11">
         <v>1</v>
       </c>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
+      <c r="D29" s="9">
+        <v>25</v>
+      </c>
+      <c r="E29" s="10">
+        <f t="shared" ref="E29:E37" si="3">D29*C29</f>
+        <v>25</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A30" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="B30" s="3">
+      <c r="B30" s="8">
         <v>43388</v>
       </c>
-      <c r="C30" s="16">
+      <c r="C30" s="11">
         <v>1</v>
       </c>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
+      <c r="D30" s="9">
+        <v>25</v>
+      </c>
+      <c r="E30" s="10">
+        <f t="shared" si="3"/>
+        <v>25</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A31" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="B31" s="3">
+      <c r="B31" s="8">
         <v>43753</v>
       </c>
-      <c r="C31" s="16">
+      <c r="C31" s="11">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
-        <v>35</v>
-      </c>
-      <c r="B32" s="3">
+      <c r="D31" s="9">
+        <v>25</v>
+      </c>
+      <c r="E31" s="10">
+        <f t="shared" si="3"/>
+        <v>12.5</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A32" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="B32" s="8">
         <v>43392</v>
       </c>
-      <c r="C32" s="16">
+      <c r="C32" s="11"/>
+      <c r="D32" s="9"/>
+      <c r="E32" s="23">
+        <f>60*0.77</f>
+        <v>46.2</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A33" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="B33" s="8">
+        <v>43392</v>
+      </c>
+      <c r="C33" s="11">
         <v>0.5</v>
       </c>
-      <c r="F32" s="4">
-        <v>35</v>
-      </c>
-      <c r="G32" s="2" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
-        <v>36</v>
-      </c>
-      <c r="B33" s="3">
-        <v>43393</v>
-      </c>
-      <c r="C33" s="16">
-        <v>0.5</v>
+      <c r="D33" s="9">
+        <v>25</v>
+      </c>
+      <c r="E33" s="10">
+        <f t="shared" si="3"/>
+        <v>12.5</v>
       </c>
       <c r="F33" s="4"/>
       <c r="G33" s="2"/>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B34" s="3"/>
-    </row>
-    <row r="35" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B35" s="23" t="s">
+      <c r="A34" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="B34" s="8">
+        <v>43393</v>
+      </c>
+      <c r="C34" s="11">
+        <v>0.5</v>
+      </c>
+      <c r="D34" s="9">
+        <v>25</v>
+      </c>
+      <c r="E34" s="10">
+        <f t="shared" si="3"/>
+        <v>12.5</v>
+      </c>
+      <c r="F34" s="4"/>
+      <c r="G34" s="2"/>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A35" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="B35" s="8">
+        <v>43395</v>
+      </c>
+      <c r="C35" s="11"/>
+      <c r="D35" s="24"/>
+      <c r="E35" s="23">
+        <v>10.98</v>
+      </c>
+      <c r="F35" s="22"/>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A36" s="7"/>
+      <c r="B36" s="8"/>
+      <c r="C36" s="11"/>
+      <c r="D36" s="24"/>
+      <c r="E36" s="25"/>
+      <c r="F36" s="22"/>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A37" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="B37" s="8">
+        <v>43395</v>
+      </c>
+      <c r="C37" s="11">
+        <v>2</v>
+      </c>
+      <c r="D37" s="9">
+        <v>25</v>
+      </c>
+      <c r="E37" s="10">
+        <f>D37*C37</f>
+        <v>50</v>
+      </c>
+      <c r="F37" s="4"/>
+      <c r="G37" s="2"/>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A38" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="B38" s="8">
+        <v>43402</v>
+      </c>
+      <c r="C38" s="11">
+        <v>0.5</v>
+      </c>
+      <c r="D38" s="9">
+        <v>25</v>
+      </c>
+      <c r="E38" s="10">
+        <f>D38*C38</f>
+        <v>12.5</v>
+      </c>
+      <c r="F38" s="4"/>
+      <c r="G38" s="2"/>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A39" s="7"/>
+      <c r="B39" s="8"/>
+      <c r="C39" s="11"/>
+      <c r="D39" s="9"/>
+      <c r="E39" s="7"/>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A40" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="B40" s="8"/>
+      <c r="C40" s="11"/>
+      <c r="D40" s="9"/>
+      <c r="E40" s="23">
+        <v>-35</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A41" s="32"/>
+      <c r="B41" s="32" t="s">
         <v>12</v>
       </c>
-      <c r="C35" s="24">
-        <f>SUM(C19:C33)</f>
-        <v>13</v>
+      <c r="C41" s="19">
+        <f>SUM(C19:C38)</f>
+        <v>15.5</v>
+      </c>
+      <c r="D41" s="19"/>
+      <c r="E41" s="19">
+        <f>SUM(E19:E39)+E40</f>
+        <v>409.68</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
started adding Henry Moore works
</commit_message>
<xml_diff>
--- a/DTA Timesheet.xlsx
+++ b/DTA Timesheet.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Derek12\Websites\DylanTaylorArt\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84DBDE83-CF1F-4209-BEA4-4C7952009BF7}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A5D8953-246B-4752-85CC-6CD1EE417360}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12810" xr2:uid="{60DF4AC3-BC03-4BD3-A93B-2AA258ECDB98}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{60DF4AC3-BC03-4BD3-A93B-2AA258ECDB98}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="2018" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="179021"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -23,6 +23,7 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -64,7 +65,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="41">
   <si>
     <t>Task</t>
   </si>
@@ -337,7 +338,7 @@
     <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -351,17 +352,6 @@
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -388,10 +378,6 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="44" fontId="4" fillId="4" borderId="1" xfId="3" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -407,6 +393,9 @@
     </xf>
     <xf numFmtId="44" fontId="5" fillId="5" borderId="1" xfId="4" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="2" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="4" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -729,302 +718,302 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FF146F9C-C34C-42C9-A414-9BE0020E9CF3}">
   <dimension ref="A1:G41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A18" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="G25" sqref="G25"/>
+    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="43.85546875" customWidth="1"/>
     <col min="2" max="2" width="14.85546875" style="2" customWidth="1"/>
-    <col min="3" max="3" width="9.140625" style="16"/>
+    <col min="3" max="3" width="9.140625" style="11"/>
     <col min="4" max="4" width="9.140625" style="6"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="12" t="s">
+      <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="13" t="s">
+      <c r="B1" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="C1" s="15" t="s">
+      <c r="C1" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="14" t="s">
+      <c r="D1" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="E1" s="12" t="s">
+      <c r="E1" s="7" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="27" t="s">
+      <c r="A2" s="20" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="28">
+      <c r="B2" s="21">
         <v>43355</v>
       </c>
-      <c r="C2" s="29">
+      <c r="C2" s="22">
         <v>0.25</v>
       </c>
-      <c r="D2" s="30">
-        <v>25</v>
-      </c>
-      <c r="E2" s="31">
+      <c r="D2" s="23">
+        <v>25</v>
+      </c>
+      <c r="E2" s="24">
         <f t="shared" ref="E2:E11" si="0">D2*C2</f>
         <v>6.25</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="27" t="s">
+      <c r="A3" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="28">
+      <c r="B3" s="21">
         <v>43355</v>
       </c>
-      <c r="C3" s="29">
+      <c r="C3" s="22">
         <v>0.1</v>
       </c>
-      <c r="D3" s="30">
-        <v>25</v>
-      </c>
-      <c r="E3" s="31">
+      <c r="D3" s="23">
+        <v>25</v>
+      </c>
+      <c r="E3" s="24">
         <f t="shared" si="0"/>
         <v>2.5</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="27" t="s">
+      <c r="A4" s="20" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="28">
+      <c r="B4" s="21">
         <v>43355</v>
       </c>
-      <c r="C4" s="29">
+      <c r="C4" s="22">
         <v>0.25</v>
       </c>
-      <c r="D4" s="30">
-        <v>25</v>
-      </c>
-      <c r="E4" s="31">
+      <c r="D4" s="23">
+        <v>25</v>
+      </c>
+      <c r="E4" s="24">
         <f t="shared" si="0"/>
         <v>6.25</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="27" t="s">
+      <c r="A5" s="20" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="28">
+      <c r="B5" s="21">
         <v>43355</v>
       </c>
-      <c r="C5" s="29">
+      <c r="C5" s="22">
         <v>0.25</v>
       </c>
-      <c r="D5" s="30">
-        <v>25</v>
-      </c>
-      <c r="E5" s="31">
+      <c r="D5" s="23">
+        <v>25</v>
+      </c>
+      <c r="E5" s="24">
         <f t="shared" si="0"/>
         <v>6.25</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="27" t="s">
+      <c r="A6" s="20" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="28">
+      <c r="B6" s="21">
         <v>43355</v>
       </c>
-      <c r="C6" s="29">
+      <c r="C6" s="22">
         <v>0.1</v>
       </c>
-      <c r="D6" s="30">
-        <v>25</v>
-      </c>
-      <c r="E6" s="31">
+      <c r="D6" s="23">
+        <v>25</v>
+      </c>
+      <c r="E6" s="24">
         <f t="shared" si="0"/>
         <v>2.5</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="27" t="s">
+      <c r="A7" s="20" t="s">
         <v>8</v>
       </c>
-      <c r="B7" s="28">
+      <c r="B7" s="21">
         <v>43355</v>
       </c>
-      <c r="C7" s="29">
+      <c r="C7" s="22">
         <v>0.25</v>
       </c>
-      <c r="D7" s="30">
-        <v>25</v>
-      </c>
-      <c r="E7" s="31">
+      <c r="D7" s="23">
+        <v>25</v>
+      </c>
+      <c r="E7" s="24">
         <f t="shared" si="0"/>
         <v>6.25</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="27" t="s">
+      <c r="A8" s="20" t="s">
         <v>9</v>
       </c>
-      <c r="B8" s="28">
+      <c r="B8" s="21">
         <v>43355</v>
       </c>
-      <c r="C8" s="29">
+      <c r="C8" s="22">
         <v>0.5</v>
       </c>
-      <c r="D8" s="30">
-        <v>25</v>
-      </c>
-      <c r="E8" s="31">
+      <c r="D8" s="23">
+        <v>25</v>
+      </c>
+      <c r="E8" s="24">
         <f t="shared" si="0"/>
         <v>12.5</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="27" t="s">
+      <c r="A9" s="20" t="s">
         <v>10</v>
       </c>
-      <c r="B9" s="28">
+      <c r="B9" s="21">
         <v>43356</v>
       </c>
-      <c r="C9" s="29">
+      <c r="C9" s="22">
         <v>2</v>
       </c>
-      <c r="D9" s="30">
-        <v>25</v>
-      </c>
-      <c r="E9" s="31">
+      <c r="D9" s="23">
+        <v>25</v>
+      </c>
+      <c r="E9" s="24">
         <f t="shared" si="0"/>
         <v>50</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="27" t="s">
+      <c r="A10" s="20" t="s">
         <v>11</v>
       </c>
-      <c r="B10" s="28">
+      <c r="B10" s="21">
         <v>43356</v>
       </c>
-      <c r="C10" s="29">
+      <c r="C10" s="22">
         <v>1</v>
       </c>
-      <c r="D10" s="30">
-        <v>25</v>
-      </c>
-      <c r="E10" s="31">
+      <c r="D10" s="23">
+        <v>25</v>
+      </c>
+      <c r="E10" s="24">
         <f t="shared" si="0"/>
         <v>25</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" s="27" t="s">
+      <c r="A11" s="20" t="s">
         <v>13</v>
       </c>
-      <c r="B11" s="28">
+      <c r="B11" s="21">
         <v>43357</v>
       </c>
-      <c r="C11" s="29">
+      <c r="C11" s="22">
         <v>1.5</v>
       </c>
-      <c r="D11" s="30">
-        <v>25</v>
-      </c>
-      <c r="E11" s="31">
+      <c r="D11" s="23">
+        <v>25</v>
+      </c>
+      <c r="E11" s="24">
         <f t="shared" si="0"/>
         <v>37.5</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" s="27" t="s">
+      <c r="A12" s="20" t="s">
         <v>14</v>
       </c>
-      <c r="B12" s="28">
+      <c r="B12" s="21">
         <v>43358</v>
       </c>
-      <c r="C12" s="29">
+      <c r="C12" s="22">
         <v>2</v>
       </c>
-      <c r="D12" s="30">
-        <v>25</v>
-      </c>
-      <c r="E12" s="31">
+      <c r="D12" s="23">
+        <v>25</v>
+      </c>
+      <c r="E12" s="24">
         <f>D12*C12</f>
         <v>50</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" s="27" t="s">
+      <c r="A13" s="20" t="s">
         <v>15</v>
       </c>
-      <c r="B13" s="28">
+      <c r="B13" s="21">
         <v>43361</v>
       </c>
-      <c r="C13" s="29">
+      <c r="C13" s="22">
         <v>2</v>
       </c>
-      <c r="D13" s="30">
-        <v>25</v>
-      </c>
-      <c r="E13" s="31">
+      <c r="D13" s="23">
+        <v>25</v>
+      </c>
+      <c r="E13" s="24">
         <f t="shared" ref="E13:E15" si="1">D13*C13</f>
         <v>50</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" s="27" t="s">
+      <c r="A14" s="20" t="s">
         <v>16</v>
       </c>
-      <c r="B14" s="28">
+      <c r="B14" s="21">
         <v>43362</v>
       </c>
-      <c r="C14" s="29">
+      <c r="C14" s="22">
         <v>1</v>
       </c>
-      <c r="D14" s="30">
-        <v>25</v>
-      </c>
-      <c r="E14" s="31">
+      <c r="D14" s="23">
+        <v>25</v>
+      </c>
+      <c r="E14" s="24">
         <f t="shared" si="1"/>
         <v>25</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" s="27" t="s">
+      <c r="A15" s="20" t="s">
         <v>17</v>
       </c>
-      <c r="B15" s="28">
+      <c r="B15" s="21">
         <v>43363</v>
       </c>
-      <c r="C15" s="29">
+      <c r="C15" s="22">
         <v>2</v>
       </c>
-      <c r="D15" s="30">
-        <v>25</v>
-      </c>
-      <c r="E15" s="31">
+      <c r="D15" s="23">
+        <v>25</v>
+      </c>
+      <c r="E15" s="24">
         <f t="shared" si="1"/>
         <v>50</v>
       </c>
     </row>
     <row r="16" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="17"/>
-      <c r="B16" s="18" t="s">
+      <c r="A16" s="12"/>
+      <c r="B16" s="13" t="s">
         <v>32</v>
       </c>
-      <c r="C16" s="19">
+      <c r="C16" s="14">
         <f>SUM(C2:C15)</f>
         <v>13.2</v>
       </c>
-      <c r="D16" s="20"/>
-      <c r="E16" s="21">
+      <c r="D16" s="15"/>
+      <c r="E16" s="16">
         <f>SUM(E2:E15)</f>
         <v>330</v>
       </c>
-      <c r="F16" s="26" t="s">
+      <c r="F16" s="19" t="s">
         <v>33</v>
       </c>
     </row>
@@ -1032,274 +1021,274 @@
       <c r="B17" s="3"/>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A18" s="12" t="s">
+      <c r="A18" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B18" s="13" t="s">
+      <c r="B18" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="C18" s="15" t="s">
+      <c r="C18" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="D18" s="14" t="s">
+      <c r="D18" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="E18" s="12" t="s">
+      <c r="E18" s="7" t="s">
         <v>31</v>
       </c>
       <c r="F18" s="5"/>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19" s="7" t="s">
+      <c r="A19" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="B19" s="8">
+      <c r="B19" s="21">
         <v>43364</v>
       </c>
-      <c r="C19" s="11">
+      <c r="C19" s="22">
         <v>1.5</v>
       </c>
-      <c r="D19" s="9">
-        <v>25</v>
-      </c>
-      <c r="E19" s="10">
+      <c r="D19" s="23">
+        <v>25</v>
+      </c>
+      <c r="E19" s="24">
         <f>D19*C19</f>
         <v>37.5</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A20" s="7" t="s">
+      <c r="A20" s="20" t="s">
         <v>19</v>
       </c>
-      <c r="B20" s="8">
+      <c r="B20" s="21">
         <v>43364</v>
       </c>
-      <c r="C20" s="11">
+      <c r="C20" s="22">
         <v>1</v>
       </c>
-      <c r="D20" s="9">
-        <v>25</v>
-      </c>
-      <c r="E20" s="10">
+      <c r="D20" s="23">
+        <v>25</v>
+      </c>
+      <c r="E20" s="24">
         <f t="shared" ref="E20:E26" si="2">D20*C20</f>
         <v>25</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A21" s="7" t="s">
+      <c r="A21" s="20" t="s">
         <v>21</v>
       </c>
-      <c r="B21" s="8">
+      <c r="B21" s="21">
         <v>43367</v>
       </c>
-      <c r="C21" s="11">
+      <c r="C21" s="22">
         <v>1</v>
       </c>
-      <c r="D21" s="9">
-        <v>25</v>
-      </c>
-      <c r="E21" s="10">
+      <c r="D21" s="23">
+        <v>25</v>
+      </c>
+      <c r="E21" s="24">
         <f t="shared" si="2"/>
         <v>25</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A22" s="7" t="s">
+      <c r="A22" s="20" t="s">
         <v>20</v>
       </c>
-      <c r="B22" s="8">
+      <c r="B22" s="21">
         <v>43368</v>
       </c>
-      <c r="C22" s="11">
+      <c r="C22" s="22">
         <v>2.5</v>
       </c>
-      <c r="D22" s="9">
-        <v>25</v>
-      </c>
-      <c r="E22" s="10">
+      <c r="D22" s="23">
+        <v>25</v>
+      </c>
+      <c r="E22" s="24">
         <f t="shared" si="2"/>
         <v>62.5</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A23" s="7" t="s">
+      <c r="A23" s="20" t="s">
         <v>22</v>
       </c>
-      <c r="B23" s="8">
+      <c r="B23" s="21">
         <v>43369</v>
       </c>
-      <c r="C23" s="11">
+      <c r="C23" s="22">
         <v>1</v>
       </c>
-      <c r="D23" s="9">
-        <v>25</v>
-      </c>
-      <c r="E23" s="10">
+      <c r="D23" s="23">
+        <v>25</v>
+      </c>
+      <c r="E23" s="24">
         <f t="shared" si="2"/>
         <v>25</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A24" s="7" t="s">
+      <c r="A24" s="20" t="s">
         <v>23</v>
       </c>
-      <c r="B24" s="8">
+      <c r="B24" s="21">
         <v>43372</v>
       </c>
-      <c r="C24" s="11">
+      <c r="C24" s="22">
         <v>0.5</v>
       </c>
-      <c r="D24" s="9">
-        <v>25</v>
-      </c>
-      <c r="E24" s="10">
+      <c r="D24" s="23">
+        <v>25</v>
+      </c>
+      <c r="E24" s="24">
         <f t="shared" si="2"/>
         <v>12.5</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A25" s="7" t="s">
+      <c r="A25" s="20" t="s">
         <v>24</v>
       </c>
-      <c r="B25" s="8">
+      <c r="B25" s="21">
         <v>43374</v>
       </c>
-      <c r="C25" s="11">
+      <c r="C25" s="22">
         <v>0.5</v>
       </c>
-      <c r="D25" s="9">
-        <v>25</v>
-      </c>
-      <c r="E25" s="10">
+      <c r="D25" s="23">
+        <v>25</v>
+      </c>
+      <c r="E25" s="24">
         <f t="shared" si="2"/>
         <v>12.5</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A26" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="B26" s="8">
+      <c r="A26" s="20" t="s">
+        <v>25</v>
+      </c>
+      <c r="B26" s="21">
         <v>43376</v>
       </c>
-      <c r="C26" s="11">
+      <c r="C26" s="22">
         <v>0.5</v>
       </c>
-      <c r="D26" s="9">
-        <v>25</v>
-      </c>
-      <c r="E26" s="10">
+      <c r="D26" s="23">
+        <v>25</v>
+      </c>
+      <c r="E26" s="24">
         <f t="shared" si="2"/>
         <v>12.5</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A27" s="7"/>
-      <c r="B27" s="8"/>
-      <c r="C27" s="11"/>
-      <c r="D27" s="9"/>
-      <c r="E27" s="7"/>
+      <c r="A27" s="20"/>
+      <c r="B27" s="21"/>
+      <c r="C27" s="22"/>
+      <c r="D27" s="23"/>
+      <c r="E27" s="20"/>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A28" s="7" t="s">
+      <c r="A28" s="20" t="s">
         <v>26</v>
       </c>
-      <c r="B28" s="8">
+      <c r="B28" s="21">
         <v>43380</v>
       </c>
-      <c r="C28" s="11">
+      <c r="C28" s="22">
         <v>1</v>
       </c>
-      <c r="D28" s="9">
-        <v>25</v>
-      </c>
-      <c r="E28" s="10">
+      <c r="D28" s="23">
+        <v>25</v>
+      </c>
+      <c r="E28" s="24">
         <f>D28*C28</f>
         <v>25</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A29" s="7" t="s">
+      <c r="A29" s="20" t="s">
         <v>27</v>
       </c>
-      <c r="B29" s="8">
+      <c r="B29" s="21">
         <v>43387</v>
       </c>
-      <c r="C29" s="11">
+      <c r="C29" s="22">
         <v>1</v>
       </c>
-      <c r="D29" s="9">
-        <v>25</v>
-      </c>
-      <c r="E29" s="10">
-        <f t="shared" ref="E29:E37" si="3">D29*C29</f>
+      <c r="D29" s="23">
+        <v>25</v>
+      </c>
+      <c r="E29" s="24">
+        <f t="shared" ref="E29:E34" si="3">D29*C29</f>
         <v>25</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A30" s="7" t="s">
+      <c r="A30" s="20" t="s">
         <v>28</v>
       </c>
-      <c r="B30" s="8">
+      <c r="B30" s="21">
         <v>43388</v>
       </c>
-      <c r="C30" s="11">
+      <c r="C30" s="22">
         <v>1</v>
       </c>
-      <c r="D30" s="9">
-        <v>25</v>
-      </c>
-      <c r="E30" s="10">
+      <c r="D30" s="23">
+        <v>25</v>
+      </c>
+      <c r="E30" s="24">
         <f t="shared" si="3"/>
         <v>25</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A31" s="7" t="s">
+      <c r="A31" s="20" t="s">
         <v>29</v>
       </c>
-      <c r="B31" s="8">
+      <c r="B31" s="21">
         <v>43753</v>
       </c>
-      <c r="C31" s="11">
+      <c r="C31" s="22">
         <v>0.5</v>
       </c>
-      <c r="D31" s="9">
-        <v>25</v>
-      </c>
-      <c r="E31" s="10">
+      <c r="D31" s="23">
+        <v>25</v>
+      </c>
+      <c r="E31" s="24">
         <f t="shared" si="3"/>
         <v>12.5</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A32" s="7" t="s">
+      <c r="A32" s="20" t="s">
         <v>38</v>
       </c>
-      <c r="B32" s="8">
+      <c r="B32" s="21">
         <v>43392</v>
       </c>
-      <c r="C32" s="11"/>
-      <c r="D32" s="9"/>
-      <c r="E32" s="23">
+      <c r="C32" s="22"/>
+      <c r="D32" s="23"/>
+      <c r="E32" s="18">
         <f>60*0.77</f>
         <v>46.2</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A33" s="7" t="s">
+      <c r="A33" s="20" t="s">
         <v>34</v>
       </c>
-      <c r="B33" s="8">
+      <c r="B33" s="21">
         <v>43392</v>
       </c>
-      <c r="C33" s="11">
+      <c r="C33" s="22">
         <v>0.5</v>
       </c>
-      <c r="D33" s="9">
-        <v>25</v>
-      </c>
-      <c r="E33" s="10">
+      <c r="D33" s="23">
+        <v>25</v>
+      </c>
+      <c r="E33" s="24">
         <f t="shared" si="3"/>
         <v>12.5</v>
       </c>
@@ -1307,19 +1296,19 @@
       <c r="G33" s="2"/>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A34" s="7" t="s">
+      <c r="A34" s="20" t="s">
         <v>35</v>
       </c>
-      <c r="B34" s="8">
+      <c r="B34" s="21">
         <v>43393</v>
       </c>
-      <c r="C34" s="11">
+      <c r="C34" s="22">
         <v>0.5</v>
       </c>
-      <c r="D34" s="9">
-        <v>25</v>
-      </c>
-      <c r="E34" s="10">
+      <c r="D34" s="23">
+        <v>25</v>
+      </c>
+      <c r="E34" s="24">
         <f t="shared" si="3"/>
         <v>12.5</v>
       </c>
@@ -1327,41 +1316,41 @@
       <c r="G34" s="2"/>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A35" s="7" t="s">
+      <c r="A35" s="20" t="s">
         <v>39</v>
       </c>
-      <c r="B35" s="8">
+      <c r="B35" s="21">
         <v>43395</v>
       </c>
-      <c r="C35" s="11"/>
-      <c r="D35" s="24"/>
-      <c r="E35" s="23">
+      <c r="C35" s="22"/>
+      <c r="D35" s="26"/>
+      <c r="E35" s="18">
         <v>10.98</v>
       </c>
-      <c r="F35" s="22"/>
+      <c r="F35" s="17"/>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A36" s="7"/>
-      <c r="B36" s="8"/>
-      <c r="C36" s="11"/>
-      <c r="D36" s="24"/>
-      <c r="E36" s="25"/>
-      <c r="F36" s="22"/>
+      <c r="A36" s="20"/>
+      <c r="B36" s="21"/>
+      <c r="C36" s="22"/>
+      <c r="D36" s="26"/>
+      <c r="E36" s="24"/>
+      <c r="F36" s="17"/>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A37" s="7" t="s">
+      <c r="A37" s="20" t="s">
         <v>36</v>
       </c>
-      <c r="B37" s="8">
+      <c r="B37" s="21">
         <v>43395</v>
       </c>
-      <c r="C37" s="11">
+      <c r="C37" s="22">
         <v>2</v>
       </c>
-      <c r="D37" s="9">
-        <v>25</v>
-      </c>
-      <c r="E37" s="10">
+      <c r="D37" s="23">
+        <v>25</v>
+      </c>
+      <c r="E37" s="24">
         <f>D37*C37</f>
         <v>50</v>
       </c>
@@ -1369,19 +1358,19 @@
       <c r="G37" s="2"/>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A38" s="7" t="s">
+      <c r="A38" s="20" t="s">
         <v>40</v>
       </c>
-      <c r="B38" s="8">
+      <c r="B38" s="21">
         <v>43402</v>
       </c>
-      <c r="C38" s="11">
+      <c r="C38" s="22">
         <v>0.5</v>
       </c>
-      <c r="D38" s="9">
-        <v>25</v>
-      </c>
-      <c r="E38" s="10">
+      <c r="D38" s="23">
+        <v>25</v>
+      </c>
+      <c r="E38" s="24">
         <f>D38*C38</f>
         <v>12.5</v>
       </c>
@@ -1389,36 +1378,39 @@
       <c r="G38" s="2"/>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A39" s="7"/>
-      <c r="B39" s="8"/>
-      <c r="C39" s="11"/>
-      <c r="D39" s="9"/>
-      <c r="E39" s="7"/>
+      <c r="A39" s="20"/>
+      <c r="B39" s="21"/>
+      <c r="C39" s="22"/>
+      <c r="D39" s="23"/>
+      <c r="E39" s="20"/>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A40" s="7" t="s">
+      <c r="A40" s="20" t="s">
         <v>37</v>
       </c>
-      <c r="B40" s="8"/>
-      <c r="C40" s="11"/>
-      <c r="D40" s="9"/>
-      <c r="E40" s="23">
+      <c r="B40" s="21"/>
+      <c r="C40" s="22"/>
+      <c r="D40" s="23"/>
+      <c r="E40" s="18">
         <v>-35</v>
       </c>
     </row>
     <row r="41" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="32"/>
-      <c r="B41" s="32" t="s">
+      <c r="A41" s="25"/>
+      <c r="B41" s="25" t="s">
         <v>12</v>
       </c>
-      <c r="C41" s="19">
+      <c r="C41" s="14">
         <f>SUM(C19:C38)</f>
         <v>15.5</v>
       </c>
-      <c r="D41" s="19"/>
-      <c r="E41" s="19">
+      <c r="D41" s="14"/>
+      <c r="E41" s="14">
         <f>SUM(E19:E39)+E40</f>
         <v>409.68</v>
+      </c>
+      <c r="F41" s="19" t="s">
+        <v>33</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Completed first draft of Henyr Moore page
</commit_message>
<xml_diff>
--- a/DTA Timesheet.xlsx
+++ b/DTA Timesheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Derek12\Websites\DylanTaylorArt\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A5D8953-246B-4752-85CC-6CD1EE417360}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7693A3BA-357F-4607-996B-8CE0496FA5A5}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{60DF4AC3-BC03-4BD3-A93B-2AA258ECDB98}"/>
   </bookViews>
@@ -65,7 +65,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="42">
   <si>
     <t>Task</t>
   </si>
@@ -188,6 +188,9 @@
   </si>
   <si>
     <t>Corrections to the data</t>
+  </si>
+  <si>
+    <t>Adding a Dropdown Menu for other artists</t>
   </si>
 </sst>
 </file>
@@ -338,7 +341,7 @@
     <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -398,6 +401,7 @@
     <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="4" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Bad" xfId="3" builtinId="27"/>
@@ -716,10 +720,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FF146F9C-C34C-42C9-A414-9BE0020E9CF3}">
-  <dimension ref="A1:G41"/>
+  <dimension ref="A1:G58"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+    <sheetView tabSelected="1" topLeftCell="A37" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="C45" sqref="C45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1413,6 +1417,199 @@
         <v>33</v>
       </c>
     </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A43" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="B43" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="C43" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="D43" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="E43" s="7" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>41</v>
+      </c>
+      <c r="B44" s="27">
+        <v>43505</v>
+      </c>
+      <c r="C44">
+        <v>1</v>
+      </c>
+      <c r="D44">
+        <v>25</v>
+      </c>
+      <c r="E44">
+        <f t="shared" ref="E44:E53" si="4">D44*C44</f>
+        <v>25</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B45"/>
+      <c r="C45"/>
+      <c r="D45">
+        <v>25</v>
+      </c>
+      <c r="E45">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B46"/>
+      <c r="C46"/>
+      <c r="D46">
+        <v>25</v>
+      </c>
+      <c r="E46">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B47"/>
+      <c r="C47"/>
+      <c r="D47">
+        <v>25</v>
+      </c>
+      <c r="E47">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B48"/>
+      <c r="C48"/>
+      <c r="D48">
+        <v>25</v>
+      </c>
+      <c r="E48">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B49"/>
+      <c r="C49"/>
+      <c r="D49">
+        <v>25</v>
+      </c>
+      <c r="E49">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B50"/>
+      <c r="C50"/>
+      <c r="D50">
+        <v>25</v>
+      </c>
+      <c r="E50">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B51"/>
+      <c r="C51"/>
+      <c r="D51">
+        <v>25</v>
+      </c>
+      <c r="E51">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B52"/>
+      <c r="C52"/>
+      <c r="D52">
+        <v>25</v>
+      </c>
+      <c r="E52">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B53"/>
+      <c r="C53"/>
+      <c r="D53">
+        <v>25</v>
+      </c>
+      <c r="E53">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B54"/>
+      <c r="C54"/>
+      <c r="D54">
+        <v>25</v>
+      </c>
+      <c r="E54">
+        <f>D54*C54</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B55"/>
+      <c r="C55"/>
+      <c r="D55">
+        <v>25</v>
+      </c>
+      <c r="E55">
+        <f t="shared" ref="E55:E57" si="5">D55*C55</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B56"/>
+      <c r="C56"/>
+      <c r="D56">
+        <v>25</v>
+      </c>
+      <c r="E56">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B57"/>
+      <c r="C57"/>
+      <c r="D57">
+        <v>25</v>
+      </c>
+      <c r="E57">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A58" s="12"/>
+      <c r="B58" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="C58" s="14">
+        <f>SUM(C44:C57)</f>
+        <v>1</v>
+      </c>
+      <c r="D58" s="15"/>
+      <c r="E58" s="16">
+        <f>SUM(E44:E57)</f>
+        <v>25</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Updated changes to Henry Moore page
</commit_message>
<xml_diff>
--- a/DTA Timesheet.xlsx
+++ b/DTA Timesheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Derek12\Websites\DylanTaylorArt\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7693A3BA-357F-4607-996B-8CE0496FA5A5}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8152F260-2BB9-4C72-AD41-4E52323E1EAA}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{60DF4AC3-BC03-4BD3-A93B-2AA258ECDB98}"/>
+    <workbookView xWindow="5580" yWindow="1260" windowWidth="22410" windowHeight="14895" xr2:uid="{60DF4AC3-BC03-4BD3-A93B-2AA258ECDB98}"/>
   </bookViews>
   <sheets>
     <sheet name="2018" sheetId="1" r:id="rId1"/>
@@ -65,7 +65,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="43">
   <si>
     <t>Task</t>
   </si>
@@ -191,6 +191,9 @@
   </si>
   <si>
     <t>Adding a Dropdown Menu for other artists</t>
+  </si>
+  <si>
+    <t>Added Henry Moore Page</t>
   </si>
 </sst>
 </file>
@@ -1453,14 +1456,21 @@
       </c>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B45"/>
-      <c r="C45"/>
+      <c r="A45" t="s">
+        <v>42</v>
+      </c>
+      <c r="B45" s="27">
+        <v>43506</v>
+      </c>
+      <c r="C45">
+        <v>0.75</v>
+      </c>
       <c r="D45">
         <v>25</v>
       </c>
       <c r="E45">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>18.75</v>
       </c>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.25">
@@ -1602,12 +1612,12 @@
       </c>
       <c r="C58" s="14">
         <f>SUM(C44:C57)</f>
-        <v>1</v>
+        <v>1.75</v>
       </c>
       <c r="D58" s="15"/>
       <c r="E58" s="16">
         <f>SUM(E44:E57)</f>
-        <v>25</v>
+        <v>43.75</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updates to the John Hoyland page
</commit_message>
<xml_diff>
--- a/DTA Timesheet.xlsx
+++ b/DTA Timesheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Derek12\Websites\DylanTaylorArt\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B5D73B1-1D3D-4978-A4E0-587FF594DB5B}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7E5E257-4A30-4724-90D6-483436BC32A4}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3735" yWindow="345" windowWidth="22410" windowHeight="14895" xr2:uid="{60DF4AC3-BC03-4BD3-A93B-2AA258ECDB98}"/>
+    <workbookView xWindow="690" yWindow="120" windowWidth="25335" windowHeight="14895" xr2:uid="{60DF4AC3-BC03-4BD3-A93B-2AA258ECDB98}"/>
   </bookViews>
   <sheets>
     <sheet name="2018" sheetId="1" r:id="rId1"/>
@@ -65,7 +65,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="46">
   <si>
     <t>Task</t>
   </si>
@@ -197,6 +197,12 @@
   </si>
   <si>
     <t>Updated Henry Moore page</t>
+  </si>
+  <si>
+    <t>Added John Hoyland page</t>
+  </si>
+  <si>
+    <t>Changes to John Hoyland page</t>
   </si>
 </sst>
 </file>
@@ -728,8 +734,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FF146F9C-C34C-42C9-A414-9BE0020E9CF3}">
   <dimension ref="A1:G58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="C47" sqref="C47"/>
+    <sheetView tabSelected="1" topLeftCell="A40" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="G48" sqref="G48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1495,25 +1501,39 @@
       </c>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B47"/>
-      <c r="C47"/>
+      <c r="A47" t="s">
+        <v>44</v>
+      </c>
+      <c r="B47" s="27">
+        <v>43514</v>
+      </c>
+      <c r="C47">
+        <v>2</v>
+      </c>
       <c r="D47">
         <v>25</v>
       </c>
       <c r="E47">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>50</v>
       </c>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B48"/>
-      <c r="C48"/>
+      <c r="A48" t="s">
+        <v>45</v>
+      </c>
+      <c r="B48" s="27">
+        <v>43515</v>
+      </c>
+      <c r="C48">
+        <v>0.3</v>
+      </c>
       <c r="D48">
         <v>25</v>
       </c>
       <c r="E48">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>7.5</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
@@ -1622,12 +1642,12 @@
       </c>
       <c r="C58" s="14">
         <f>SUM(C44:C57)</f>
-        <v>2</v>
+        <v>4.3</v>
       </c>
       <c r="D58" s="15"/>
       <c r="E58" s="16">
         <f>SUM(E44:E57)</f>
-        <v>50</v>
+        <v>107.5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added sonial delaunay and other pictures
</commit_message>
<xml_diff>
--- a/DTA Timesheet.xlsx
+++ b/DTA Timesheet.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21425"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Derek12\Websites\DylanTaylorArt\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7E5E257-4A30-4724-90D6-483436BC32A4}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00EA8275-76C9-4268-8200-4C78EF5C1B82}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="690" yWindow="120" windowWidth="25335" windowHeight="14895" xr2:uid="{60DF4AC3-BC03-4BD3-A93B-2AA258ECDB98}"/>
+    <workbookView xWindow="1380" yWindow="810" windowWidth="25335" windowHeight="14895" xr2:uid="{60DF4AC3-BC03-4BD3-A93B-2AA258ECDB98}"/>
   </bookViews>
   <sheets>
     <sheet name="2018" sheetId="1" r:id="rId1"/>
@@ -732,10 +732,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FF146F9C-C34C-42C9-A414-9BE0020E9CF3}">
-  <dimension ref="A1:G58"/>
+  <dimension ref="A1:G50"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A40" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="G48" sqref="G48"/>
+      <selection activeCell="F50" sqref="F50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1459,8 +1459,8 @@
       <c r="D44">
         <v>25</v>
       </c>
-      <c r="E44">
-        <f t="shared" ref="E44:E53" si="4">D44*C44</f>
+      <c r="E44" s="4">
+        <f t="shared" ref="E44:E48" si="4">D44*C44</f>
         <v>25</v>
       </c>
     </row>
@@ -1477,7 +1477,7 @@
       <c r="D45">
         <v>25</v>
       </c>
-      <c r="E45">
+      <c r="E45" s="4">
         <f t="shared" si="4"/>
         <v>18.75</v>
       </c>
@@ -1495,7 +1495,7 @@
       <c r="D46">
         <v>25</v>
       </c>
-      <c r="E46">
+      <c r="E46" s="4">
         <f t="shared" si="4"/>
         <v>6.25</v>
       </c>
@@ -1513,7 +1513,7 @@
       <c r="D47">
         <v>25</v>
       </c>
-      <c r="E47">
+      <c r="E47" s="4">
         <f t="shared" si="4"/>
         <v>50</v>
       </c>
@@ -1531,7 +1531,7 @@
       <c r="D48">
         <v>25</v>
       </c>
-      <c r="E48">
+      <c r="E48" s="4">
         <f t="shared" si="4"/>
         <v>7.5</v>
       </c>
@@ -1539,114 +1539,20 @@
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B49"/>
       <c r="C49"/>
-      <c r="D49">
-        <v>25</v>
-      </c>
-      <c r="E49">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B50"/>
-      <c r="C50"/>
-      <c r="D50">
-        <v>25</v>
-      </c>
-      <c r="E50">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B51"/>
-      <c r="C51"/>
-      <c r="D51">
-        <v>25</v>
-      </c>
-      <c r="E51">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B52"/>
-      <c r="C52"/>
-      <c r="D52">
-        <v>25</v>
-      </c>
-      <c r="E52">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B53"/>
-      <c r="C53"/>
-      <c r="D53">
-        <v>25</v>
-      </c>
-      <c r="E53">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B54"/>
-      <c r="C54"/>
-      <c r="D54">
-        <v>25</v>
-      </c>
-      <c r="E54">
-        <f>D54*C54</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B55"/>
-      <c r="C55"/>
-      <c r="D55">
-        <v>25</v>
-      </c>
-      <c r="E55">
-        <f t="shared" ref="E55:E57" si="5">D55*C55</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B56"/>
-      <c r="C56"/>
-      <c r="D56">
-        <v>25</v>
-      </c>
-      <c r="E56">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B57"/>
-      <c r="C57"/>
-      <c r="D57">
-        <v>25</v>
-      </c>
-      <c r="E57">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="58" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A58" s="12"/>
-      <c r="B58" s="13" t="s">
+      <c r="D49"/>
+    </row>
+    <row r="50" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A50" s="12"/>
+      <c r="B50" s="13" t="s">
         <v>32</v>
       </c>
-      <c r="C58" s="14">
-        <f>SUM(C44:C57)</f>
+      <c r="C50" s="14">
+        <f>SUM(C44:C49)</f>
         <v>4.3</v>
       </c>
-      <c r="D58" s="15"/>
-      <c r="E58" s="16">
-        <f>SUM(E44:E57)</f>
+      <c r="D50" s="15"/>
+      <c r="E50" s="16">
+        <f>SUM(E44:E49)</f>
         <v>107.5</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added more art for Delaunay and Miro
</commit_message>
<xml_diff>
--- a/DTA Timesheet.xlsx
+++ b/DTA Timesheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Derek12\Websites\DylanTaylorArt\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00EA8275-76C9-4268-8200-4C78EF5C1B82}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B45A8306-9915-4322-A2B9-E728B612F155}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1380" yWindow="810" windowWidth="25335" windowHeight="14895" xr2:uid="{60DF4AC3-BC03-4BD3-A93B-2AA258ECDB98}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{60DF4AC3-BC03-4BD3-A93B-2AA258ECDB98}"/>
   </bookViews>
   <sheets>
     <sheet name="2018" sheetId="1" r:id="rId1"/>
@@ -65,7 +65,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="47">
   <si>
     <t>Task</t>
   </si>
@@ -203,6 +203,9 @@
   </si>
   <si>
     <t>Changes to John Hoyland page</t>
+  </si>
+  <si>
+    <t>Added Sonia Delaunay + Henry Moore</t>
   </si>
 </sst>
 </file>
@@ -353,7 +356,7 @@
     <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -414,6 +417,12 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="4"/>
+    <xf numFmtId="14" fontId="5" fillId="5" borderId="0" xfId="4" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="4" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="5" fillId="5" borderId="0" xfId="4" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Bad" xfId="3" builtinId="27"/>
@@ -732,10 +741,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FF146F9C-C34C-42C9-A414-9BE0020E9CF3}">
-  <dimension ref="A1:G50"/>
+  <dimension ref="A1:G59"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="F50" sqref="F50"/>
+    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="H43" sqref="H43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1447,101 +1456,101 @@
       </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A44" t="s">
+      <c r="A44" s="28" t="s">
         <v>41</v>
       </c>
-      <c r="B44" s="27">
+      <c r="B44" s="29">
         <v>43505</v>
       </c>
-      <c r="C44">
+      <c r="C44" s="30">
         <v>1</v>
       </c>
-      <c r="D44">
-        <v>25</v>
-      </c>
-      <c r="E44" s="4">
+      <c r="D44" s="30">
+        <v>25</v>
+      </c>
+      <c r="E44" s="31">
         <f t="shared" ref="E44:E48" si="4">D44*C44</f>
         <v>25</v>
       </c>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A45" t="s">
+      <c r="A45" s="28" t="s">
         <v>42</v>
       </c>
-      <c r="B45" s="27">
+      <c r="B45" s="29">
         <v>43506</v>
       </c>
-      <c r="C45">
+      <c r="C45" s="30">
         <v>0.75</v>
       </c>
-      <c r="D45">
-        <v>25</v>
-      </c>
-      <c r="E45" s="4">
+      <c r="D45" s="30">
+        <v>25</v>
+      </c>
+      <c r="E45" s="31">
         <f t="shared" si="4"/>
         <v>18.75</v>
       </c>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A46" t="s">
+      <c r="A46" s="28" t="s">
         <v>43</v>
       </c>
-      <c r="B46" s="27">
+      <c r="B46" s="29">
         <v>43506</v>
       </c>
-      <c r="C46">
+      <c r="C46" s="30">
         <v>0.25</v>
       </c>
-      <c r="D46">
-        <v>25</v>
-      </c>
-      <c r="E46" s="4">
+      <c r="D46" s="30">
+        <v>25</v>
+      </c>
+      <c r="E46" s="31">
         <f t="shared" si="4"/>
         <v>6.25</v>
       </c>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A47" t="s">
+      <c r="A47" s="28" t="s">
         <v>44</v>
       </c>
-      <c r="B47" s="27">
+      <c r="B47" s="29">
         <v>43514</v>
       </c>
-      <c r="C47">
+      <c r="C47" s="30">
         <v>2</v>
       </c>
-      <c r="D47">
-        <v>25</v>
-      </c>
-      <c r="E47" s="4">
+      <c r="D47" s="30">
+        <v>25</v>
+      </c>
+      <c r="E47" s="31">
         <f t="shared" si="4"/>
         <v>50</v>
       </c>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A48" t="s">
+      <c r="A48" s="28" t="s">
         <v>45</v>
       </c>
-      <c r="B48" s="27">
+      <c r="B48" s="29">
         <v>43515</v>
       </c>
-      <c r="C48">
+      <c r="C48" s="30">
         <v>0.3</v>
       </c>
-      <c r="D48">
-        <v>25</v>
-      </c>
-      <c r="E48" s="4">
+      <c r="D48" s="30">
+        <v>25</v>
+      </c>
+      <c r="E48" s="31">
         <f t="shared" si="4"/>
         <v>7.5</v>
       </c>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B49"/>
-      <c r="C49"/>
-      <c r="D49"/>
-    </row>
-    <row r="50" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C49" s="2"/>
+      <c r="D49" s="2"/>
+    </row>
+    <row r="50" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A50" s="12"/>
       <c r="B50" s="13" t="s">
         <v>32</v>
@@ -1554,6 +1563,100 @@
       <c r="E50" s="16">
         <f>SUM(E44:E49)</f>
         <v>107.5</v>
+      </c>
+      <c r="F50" s="19" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A52" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="B52" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="C52" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="D52" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="E52" s="7" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>46</v>
+      </c>
+      <c r="B53" s="27">
+        <v>43572</v>
+      </c>
+      <c r="C53" s="2">
+        <v>1</v>
+      </c>
+      <c r="D53" s="2">
+        <v>25</v>
+      </c>
+      <c r="E53" s="4">
+        <f t="shared" ref="E53:E57" si="5">D53*C53</f>
+        <v>25</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B54" s="27"/>
+      <c r="C54" s="2"/>
+      <c r="D54" s="2"/>
+      <c r="E54" s="4">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B55" s="27"/>
+      <c r="C55" s="2"/>
+      <c r="D55" s="2"/>
+      <c r="E55" s="4">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B56" s="27"/>
+      <c r="C56" s="2"/>
+      <c r="D56" s="2"/>
+      <c r="E56" s="4">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B57" s="27"/>
+      <c r="C57" s="2"/>
+      <c r="D57" s="2"/>
+      <c r="E57" s="4">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B58"/>
+      <c r="C58" s="2"/>
+      <c r="D58" s="2"/>
+    </row>
+    <row r="59" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A59" s="12"/>
+      <c r="B59" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="C59" s="14">
+        <f>SUM(C53:C58)</f>
+        <v>1</v>
+      </c>
+      <c r="D59" s="15"/>
+      <c r="E59" s="16">
+        <f>SUM(E53:E58)</f>
+        <v>25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated other artists pictures
</commit_message>
<xml_diff>
--- a/DTA Timesheet.xlsx
+++ b/DTA Timesheet.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Derek12\Websites\DylanTaylorArt\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B45A8306-9915-4322-A2B9-E728B612F155}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D2A92EC-4998-4B2A-A31D-F3F53C1C4C02}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{60DF4AC3-BC03-4BD3-A93B-2AA258ECDB98}"/>
   </bookViews>
@@ -65,7 +65,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="49">
   <si>
     <t>Task</t>
   </si>
@@ -206,6 +206,12 @@
   </si>
   <si>
     <t>Added Sonia Delaunay + Henry Moore</t>
+  </si>
+  <si>
+    <t>Added 3rd Sonia Delaunay</t>
+  </si>
+  <si>
+    <t>Added Miro Prints</t>
   </si>
 </sst>
 </file>
@@ -743,8 +749,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FF146F9C-C34C-42C9-A414-9BE0020E9CF3}">
   <dimension ref="A1:G59"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="H43" sqref="H43"/>
+    <sheetView tabSelected="1" topLeftCell="A40" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="D56" sqref="D56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1604,21 +1610,39 @@
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B54" s="27"/>
-      <c r="C54" s="2"/>
-      <c r="D54" s="2"/>
+      <c r="A54" t="s">
+        <v>47</v>
+      </c>
+      <c r="B54" s="27">
+        <v>43731</v>
+      </c>
+      <c r="C54" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="D54" s="2">
+        <v>25</v>
+      </c>
       <c r="E54" s="4">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>12.5</v>
       </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B55" s="27"/>
-      <c r="C55" s="2"/>
-      <c r="D55" s="2"/>
+      <c r="A55" t="s">
+        <v>48</v>
+      </c>
+      <c r="B55" s="27">
+        <v>43731</v>
+      </c>
+      <c r="C55" s="2">
+        <v>2</v>
+      </c>
+      <c r="D55" s="2">
+        <v>25</v>
+      </c>
       <c r="E55" s="4">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>50</v>
       </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.25">
@@ -1651,12 +1675,12 @@
       </c>
       <c r="C59" s="14">
         <f>SUM(C53:C58)</f>
-        <v>1</v>
+        <v>3.5</v>
       </c>
       <c r="D59" s="15"/>
       <c r="E59" s="16">
         <f>SUM(E53:E58)</f>
-        <v>25</v>
+        <v>87.5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Start using the status of a graphic
</commit_message>
<xml_diff>
--- a/DTA Timesheet.xlsx
+++ b/DTA Timesheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Derek12\Websites\DylanTaylorArt\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D2A92EC-4998-4B2A-A31D-F3F53C1C4C02}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{165B530F-C433-494F-AC53-A19EE8E32415}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{60DF4AC3-BC03-4BD3-A93B-2AA258ECDB98}"/>
+    <workbookView xWindow="3345" yWindow="795" windowWidth="22755" windowHeight="14895" xr2:uid="{60DF4AC3-BC03-4BD3-A93B-2AA258ECDB98}"/>
   </bookViews>
   <sheets>
     <sheet name="2018" sheetId="1" r:id="rId1"/>
@@ -65,7 +65,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="51">
   <si>
     <t>Task</t>
   </si>
@@ -212,6 +212,12 @@
   </si>
   <si>
     <t>Added Miro Prints</t>
+  </si>
+  <si>
+    <t>Added Miro Prints plus updates</t>
+  </si>
+  <si>
+    <t>Renewal of Website Hosting</t>
   </si>
 </sst>
 </file>
@@ -749,8 +755,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FF146F9C-C34C-42C9-A414-9BE0020E9CF3}">
   <dimension ref="A1:G59"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="D56" sqref="D56"/>
+    <sheetView tabSelected="1" topLeftCell="A46" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="E57" sqref="E57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1646,21 +1652,39 @@
       </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B56" s="27"/>
-      <c r="C56" s="2"/>
-      <c r="D56" s="2"/>
+      <c r="A56" t="s">
+        <v>49</v>
+      </c>
+      <c r="B56" s="27">
+        <v>43734</v>
+      </c>
+      <c r="C56" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="D56" s="2">
+        <v>25</v>
+      </c>
       <c r="E56" s="4">
         <f t="shared" si="5"/>
+        <v>12.5</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>50</v>
+      </c>
+      <c r="B57" s="27">
+        <v>43734</v>
+      </c>
+      <c r="C57" s="2">
         <v>0</v>
       </c>
-    </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B57" s="27"/>
-      <c r="C57" s="2"/>
-      <c r="D57" s="2"/>
+      <c r="D57" s="2">
+        <v>0</v>
+      </c>
       <c r="E57" s="4">
-        <f t="shared" si="5"/>
-        <v>0</v>
+        <f>(59.4+19.95)*0.81</f>
+        <v>64.273499999999999</v>
       </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.25">
@@ -1675,12 +1699,12 @@
       </c>
       <c r="C59" s="14">
         <f>SUM(C53:C58)</f>
-        <v>3.5</v>
+        <v>4</v>
       </c>
       <c r="D59" s="15"/>
       <c r="E59" s="16">
         <f>SUM(E53:E58)</f>
-        <v>87.5</v>
+        <v>164.27350000000001</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added two Picasso prints
</commit_message>
<xml_diff>
--- a/DTA Timesheet.xlsx
+++ b/DTA Timesheet.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Derek12\Websites\DylanTaylorArt\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{165B530F-C433-494F-AC53-A19EE8E32415}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03EE3336-4428-4CFC-B0F2-395CB23A9599}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3345" yWindow="795" windowWidth="22755" windowHeight="14895" xr2:uid="{60DF4AC3-BC03-4BD3-A93B-2AA258ECDB98}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{60DF4AC3-BC03-4BD3-A93B-2AA258ECDB98}"/>
   </bookViews>
   <sheets>
     <sheet name="2018" sheetId="1" r:id="rId1"/>
@@ -65,7 +65,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="54">
   <si>
     <t>Task</t>
   </si>
@@ -218,6 +218,15 @@
   </si>
   <si>
     <t>Renewal of Website Hosting</t>
+  </si>
+  <si>
+    <t>Skype Session</t>
+  </si>
+  <si>
+    <t>Attempts at Image Orientation</t>
+  </si>
+  <si>
+    <t>Changing Price display</t>
   </si>
 </sst>
 </file>
@@ -753,10 +762,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FF146F9C-C34C-42C9-A414-9BE0020E9CF3}">
-  <dimension ref="A1:G59"/>
+  <dimension ref="A1:G63"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A46" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="E57" sqref="E57"/>
+      <selection activeCell="D62" sqref="D62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1611,7 +1620,7 @@
         <v>25</v>
       </c>
       <c r="E53" s="4">
-        <f t="shared" ref="E53:E57" si="5">D53*C53</f>
+        <f t="shared" ref="E53:E61" si="5">D53*C53</f>
         <v>25</v>
       </c>
     </row>
@@ -1688,23 +1697,96 @@
       </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B58"/>
-      <c r="C58" s="2"/>
-      <c r="D58" s="2"/>
-    </row>
-    <row r="59" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A59" s="12"/>
-      <c r="B59" s="13" t="s">
+      <c r="A58" t="s">
+        <v>51</v>
+      </c>
+      <c r="B58" s="27">
+        <v>43743</v>
+      </c>
+      <c r="C58" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="D58" s="2">
+        <v>25</v>
+      </c>
+      <c r="E58" s="4">
+        <f t="shared" si="5"/>
+        <v>12.5</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>52</v>
+      </c>
+      <c r="B59" s="27">
+        <v>43744</v>
+      </c>
+      <c r="C59" s="2">
+        <v>1</v>
+      </c>
+      <c r="D59" s="2">
+        <v>25</v>
+      </c>
+      <c r="E59" s="4">
+        <f t="shared" si="5"/>
+        <v>25</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>51</v>
+      </c>
+      <c r="B60" s="27">
+        <v>43753</v>
+      </c>
+      <c r="C60" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="D60" s="2">
+        <v>25</v>
+      </c>
+      <c r="E60" s="4">
+        <f t="shared" si="5"/>
+        <v>12.5</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
+        <v>53</v>
+      </c>
+      <c r="B61" s="27">
+        <v>43753</v>
+      </c>
+      <c r="C61" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="D61" s="2">
+        <v>25</v>
+      </c>
+      <c r="E61" s="4">
+        <f t="shared" si="5"/>
+        <v>12.5</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B62" s="27"/>
+      <c r="C62" s="2"/>
+      <c r="D62" s="2"/>
+      <c r="E62" s="4"/>
+    </row>
+    <row r="63" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A63" s="12"/>
+      <c r="B63" s="13" t="s">
         <v>32</v>
       </c>
-      <c r="C59" s="14">
-        <f>SUM(C53:C58)</f>
-        <v>4</v>
-      </c>
-      <c r="D59" s="15"/>
-      <c r="E59" s="16">
-        <f>SUM(E53:E58)</f>
-        <v>164.27350000000001</v>
+      <c r="C63" s="14">
+        <f>SUM(C53:C61)</f>
+        <v>6.5</v>
+      </c>
+      <c r="D63" s="15"/>
+      <c r="E63" s="16">
+        <f>SUM(E53:E61)</f>
+        <v>226.77350000000001</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated and moved timesheet
</commit_message>
<xml_diff>
--- a/DTA Timesheet.xlsx
+++ b/DTA Timesheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Derek12\Websites\DylanTaylorArt\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03EE3336-4428-4CFC-B0F2-395CB23A9599}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8612B6F-C582-4AD6-B778-302702E4B343}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{60DF4AC3-BC03-4BD3-A93B-2AA258ECDB98}"/>
   </bookViews>
@@ -65,7 +65,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="55">
   <si>
     <t>Task</t>
   </si>
@@ -227,6 +227,9 @@
   </si>
   <si>
     <t>Changing Price display</t>
+  </si>
+  <si>
+    <t>Added Picasso page</t>
   </si>
 </sst>
 </file>
@@ -762,7 +765,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FF146F9C-C34C-42C9-A414-9BE0020E9CF3}">
-  <dimension ref="A1:G63"/>
+  <dimension ref="A1:G64"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A46" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
       <selection activeCell="D62" sqref="D62"/>
@@ -1620,7 +1623,7 @@
         <v>25</v>
       </c>
       <c r="E53" s="4">
-        <f t="shared" ref="E53:E61" si="5">D53*C53</f>
+        <f t="shared" ref="E53:E62" si="5">D53*C53</f>
         <v>25</v>
       </c>
     </row>
@@ -1769,24 +1772,42 @@
       </c>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B62" s="27"/>
-      <c r="C62" s="2"/>
-      <c r="D62" s="2"/>
-      <c r="E62" s="4"/>
-    </row>
-    <row r="63" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A63" s="12"/>
-      <c r="B63" s="13" t="s">
+      <c r="A62" t="s">
+        <v>54</v>
+      </c>
+      <c r="B62" s="27">
+        <v>43758</v>
+      </c>
+      <c r="C62" s="2">
+        <v>1.5</v>
+      </c>
+      <c r="D62" s="2">
+        <v>25</v>
+      </c>
+      <c r="E62" s="4">
+        <f t="shared" si="5"/>
+        <v>37.5</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B63" s="27"/>
+      <c r="C63" s="2"/>
+      <c r="D63" s="2"/>
+      <c r="E63" s="4"/>
+    </row>
+    <row r="64" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A64" s="12"/>
+      <c r="B64" s="13" t="s">
         <v>32</v>
       </c>
-      <c r="C63" s="14">
-        <f>SUM(C53:C61)</f>
-        <v>6.5</v>
-      </c>
-      <c r="D63" s="15"/>
-      <c r="E63" s="16">
-        <f>SUM(E53:E61)</f>
-        <v>226.77350000000001</v>
+      <c r="C64" s="14">
+        <f>SUM(C53:C62)</f>
+        <v>8</v>
+      </c>
+      <c r="D64" s="15"/>
+      <c r="E64" s="16">
+        <f>SUM(E53:E62)</f>
+        <v>264.27350000000001</v>
       </c>
     </row>
   </sheetData>

</xml_diff>